<commit_message>
Task: Provide original location in response
* Split address is removed from response
* Response to contain uncleaned original address
</commit_message>
<xml_diff>
--- a/data/Data_AM_Accreditation(Address).xlsx
+++ b/data/Data_AM_Accreditation(Address).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IntelligentB2BMatchmaking\DataPreprocessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lekisha/PycharmProjects/Academic/b2b/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F920BEE-0883-4704-88CD-B70ED183B61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5485333A-927F-4346-888B-5C40300E60C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23240" windowHeight="13880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="1773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="2043">
   <si>
     <t>CompanyID</t>
   </si>
@@ -5364,13 +5364,823 @@
   </si>
   <si>
     <t>University of New Brunswick</t>
+  </si>
+  <si>
+    <t>Actual Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000 Simcoe Street North Oshawa L1G 7V9 Canada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">131 Citation Drive Units 17 &amp; 18 Concord L4K 2R3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1957 Turner Ave Rossland V0G 1Y0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">540 Mara Road  Beaverton Canada L0K1A0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 College Blvd., Box 5005 Red Deer T4N 5H5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">347 Jane Street Toronto M6S 3Z3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4100A Sladeview Crescent Mississauga L5L 5Z3 </t>
+  </si>
+  <si>
+    <t>9494 Boulevard Saint-Laurent Suite 600 Montreal Quebec QC H2N 1P4 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119 Hillsdale Ave West Toronto M5P 1G6 </t>
+  </si>
+  <si>
+    <t>6956, rue Jarry Est Saint-Léonard H1P 3C1 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">620 Cathcart Montreal H3B 3C4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 International Blvd. Unit 1 M9W 1A2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3095, Westinghouse Trois-Rivières G9A 5E1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 Palladium Dr Ottawa K2V 1C2 </t>
+  </si>
+  <si>
+    <t>202 6 Ave SW Calgary T2L 1Y8 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 Commerce Crescent North Bay P1A0B4 </t>
+  </si>
+  <si>
+    <t>4 - 585 Michigan Drive Oakville Ontario L6L 0G1 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2070 Fasan Drive Oldcastle N0R1L0 </t>
+  </si>
+  <si>
+    <t>1100 Avenue Atwater, Suite 3000 Westmount H3Z 2Y4 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">845 Sherbrooke St W, Montreal H3A 0G4 </t>
+  </si>
+  <si>
+    <t>36 Fieldway Rd 3rd Floor Etobicoke ON M8Z 3L2 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 Spadina Avenue, Suite 600 Toronto M5V2K4 </t>
+  </si>
+  <si>
+    <t>200 University Ave W Waterloo N2L 3G1 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office 390 55, rue de Louvain Ouest Montreal Canada H2N 1A4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4655 G.N. Booth Drive Windsor N9C 4G8 </t>
+  </si>
+  <si>
+    <t>Park - #301, 175 Longwood Rd S, Hamilton, ON L8P 0A1 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 Rue de l'Atmosphère Gatineau Canada J9A 2W5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">285 Dundas St W Toronto Canada M5T1G1 </t>
+  </si>
+  <si>
+    <t>1595 Buffalo Place Unit A Winnipeg Manitoba MB R3T1L9 Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">720, rue Longpré Sherbrooke J1G 4L3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2767 Brighton Rd. Oakville L6H 6J4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6260 Highway 7 Unit 8 Vaughan Canada L4H 4G3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 Ch. De L'Aéroport Saint-Jean-Sur-Richelieu J3B 7B5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 College Blvd Red Deer T4N 5H5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">302 Carlaw Unit 108 Toronto Canada M4M3L1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11A Rue du Pacifique E Bromont J2L 1J4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1301 16 Ave. NW. Calgary Canada T2M 0L4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vancouver V6T 1Z4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">190 Maple Hills Ave Charlottetown C1C 1N2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Dineen Drive Head Hall  Building Room E-45A Fredericton Canada E3B5A3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 King's College Cir Toronto M5S 1A1 </t>
+  </si>
+  <si>
+    <t>11th Hour Prototypes Bidford on Avon Warwickshire B50 4JH United Kingdom</t>
+  </si>
+  <si>
+    <t>Hurst End Farm Folly Ln  Newport Pagnell  MK16 9HS Buckinghamshire</t>
+  </si>
+  <si>
+    <t>Unit 1 Carlton Court Grainger Road Southend On Sea Essex  SS2 5BZ United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> North Industrial Estate 45 Drumhead Rd Chorley  PR6 0BL Lancashire</t>
+  </si>
+  <si>
+    <t>SW19 City of London</t>
+  </si>
+  <si>
+    <t>cb22 4nj Cambridgeshire</t>
+  </si>
+  <si>
+    <t>RG14 1JB Berkshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NormacotRoad Longton Stoke-On-Trent Staffordshire ST13 1PR </t>
+  </si>
+  <si>
+    <t>Nasmyth Building Nasmyth Avenue East Kilbride G75 0QR UK</t>
+  </si>
+  <si>
+    <t>32 Parton Road Aylesbury Bucks HP20 1NG UK</t>
+  </si>
+  <si>
+    <t>Unit 3A Stafford Park 16 Telford Shropshire TF3 3BS UK</t>
+  </si>
+  <si>
+    <t>Mark Road  Hemel Hempstead HP2 7UA Hertfordshire</t>
+  </si>
+  <si>
+    <t>4 Acol Court Acol Road London NW6 3AE UK</t>
+  </si>
+  <si>
+    <t>Units 7 &amp; 8 Suite 10 Elizabeth Industrial Estate, Juno Way London SE14 5RW UK</t>
+  </si>
+  <si>
+    <t>Fulton Court Wofford Way Greenham Business Park Newbury RG19 6HD Bershire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ll ll </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Mornington Road Birmingham B66 2JE </t>
+  </si>
+  <si>
+    <t>213 Torrington Avenue Tile Hill Coventry West Midlands CV4 9HN West Midlands</t>
+  </si>
+  <si>
+    <t>COATES BUILDING UNIVERSITY PARK NOTTINGHAM NG7 2RD UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>S60 5WG South Yorkshire</t>
+  </si>
+  <si>
+    <t>UNIT N EUROPA HOUSE SHEFFIELD AIRPORT BUSINESS PARK SHEFFIELD S9 1XU ENGLAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iHub - Infinity Park Innovation Way Derby Derbyshire DE24 9FU </t>
+  </si>
+  <si>
+    <t>EC2Y 9DT City of London</t>
+  </si>
+  <si>
+    <t>37 Royal Avenue Calcot Reading Berkshire RG31 4UR UK</t>
+  </si>
+  <si>
+    <t>PA4 9LJ Renfrewshire</t>
+  </si>
+  <si>
+    <t>SK5 7ER Greater Manchester</t>
+  </si>
+  <si>
+    <t>MK46 5EQ Buckinghamshire</t>
+  </si>
+  <si>
+    <t>OX2 6NA Oxfordshire</t>
+  </si>
+  <si>
+    <t>B60 3DX Worcestershire</t>
+  </si>
+  <si>
+    <t>crossgate road park farm  industrial estate Redditch Worecestershire B987TD United KIngdom</t>
+  </si>
+  <si>
+    <t>c/o Outfit Unit 5B Chester Retail Park Sealand Road Chester CH1 4RY UK</t>
+  </si>
+  <si>
+    <t>2000 Manton Ln Bedford MK41 7PF UK</t>
+  </si>
+  <si>
+    <t>SK7 2BE Greater Manchester</t>
+  </si>
+  <si>
+    <t>B15 2TT West Midlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FactoryoftheFuture AdvancedManufacturingPark WallisWayCatcliffeRotherhamS605TZ S60 5TZ </t>
+  </si>
+  <si>
+    <t>Ansty Business Park Coventry United Kingdom</t>
+  </si>
+  <si>
+    <t>DD9 6DY Angus</t>
+  </si>
+  <si>
+    <t>S9 1XH South Yorkshire</t>
+  </si>
+  <si>
+    <t>ADVANCED PIPE INSPECTION UK LTD Friar Gate Studios Ford Street Derby DE1 1EE United Kingdom</t>
+  </si>
+  <si>
+    <t>CV34 6RH Warwickshire</t>
+  </si>
+  <si>
+    <t>ROYSTON HOUSE 267 CRANMORE BOULEVARD SHIRLEY SOLIHULL WEST MIDLANDS B90 4QT UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>Unit 75 Greenfield Business Centre Greenfield Holywell Flintshire CH8 7GR UK</t>
+  </si>
+  <si>
+    <t>371 Coleford Road Sheffield S9 5NF United Kingdom</t>
+  </si>
+  <si>
+    <t>B10 0HJ West Midlands</t>
+  </si>
+  <si>
+    <t>E3 3TZ City of London</t>
+  </si>
+  <si>
+    <t>The Priestley Centre Surrey Research Park,10 Priestley Road Guildford Surrey GU2 7XY UK</t>
+  </si>
+  <si>
+    <t>Springwood Court,Springwood Close Tytherington Business Park Macclesfield Cheshire SK10 2XF UK</t>
+  </si>
+  <si>
+    <t>CH2 3AD Cheshire</t>
+  </si>
+  <si>
+    <t>The Building Centre 26 Store Street London WC1E 7BT UK</t>
+  </si>
+  <si>
+    <t>PE28 0LP Cambridgeshire</t>
+  </si>
+  <si>
+    <t>CB2 1TN Cambridgeshire</t>
+  </si>
+  <si>
+    <t>Woodhatch Reigate Surrey RH2 8BF UK</t>
+  </si>
+  <si>
+    <t>Parsons Lane Sheffield S33 6RB United Kinfdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit9WildmoorMill MillLane Wildmoor Bromsgrove, Worcestershire B61 0BX </t>
+  </si>
+  <si>
+    <t>City, University of London Northampton Square  Clerkenwell London  EC1V 0HB United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 abc road SW12 2BG </t>
+  </si>
+  <si>
+    <t>LE11 5GW Leicestershire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College Road Cranfield MK43 0AL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">520EskdaleRoadWinnershTriangleWokinghamBerkshireRG415TU RG41 5TU </t>
+  </si>
+  <si>
+    <t>Unit 20 Chorley Central Business Park Chorley PR6 0LP United Kingdom</t>
+  </si>
+  <si>
+    <t>WA3 6BL Greater Manchester</t>
+  </si>
+  <si>
+    <t>61-63 Rochester Place London NW1 9JU UK</t>
+  </si>
+  <si>
+    <t>CB5 8UZ Cambridgeshire</t>
+  </si>
+  <si>
+    <t>Armytage Road Armytage Road West Yorkshire HD6 1QF UK</t>
+  </si>
+  <si>
+    <t>CV3 4PE West Midlands</t>
+  </si>
+  <si>
+    <t>42 Basepoint Business Centre Harts Farm Way Havant Hampshire PO9 1HS UK</t>
+  </si>
+  <si>
+    <t>Workspace House 28-29 Maxwell Rd Peterborough PE2 7JE UK</t>
+  </si>
+  <si>
+    <t>Unit 56 Monument Business Park Chalgrove Oxfordshire OX44 7RW UK</t>
+  </si>
+  <si>
+    <t>CV4 7BB West Midlands</t>
+  </si>
+  <si>
+    <t>NE6 1AS Tyne and Wear</t>
+  </si>
+  <si>
+    <t>TF2 9TX Shropshire</t>
+  </si>
+  <si>
+    <t>AB12 3LY Aberdeen City</t>
+  </si>
+  <si>
+    <t>Unit 19, Laker Road Rochester Kent ME1 3QX United KIngdom</t>
+  </si>
+  <si>
+    <t>B63 2RH West Midlands</t>
+  </si>
+  <si>
+    <t>KA9 2TU South Ayrshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Homestead Watling St Towcester Northants NN12 6LH </t>
+  </si>
+  <si>
+    <t>Chaffinch Business Park Croydon Road Beckenham Kent BR3 4DW UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34SabreClose GreenFarm Quedgeley Gloucester, Gloucestershire GL2 4NZ </t>
+  </si>
+  <si>
+    <t>MK8 0JP Buckinghamshire</t>
+  </si>
+  <si>
+    <t>29-39 Brunswick Square Bloomsbury London WC1N 1AX UK</t>
+  </si>
+  <si>
+    <t>RG24 7NG Hampshire</t>
+  </si>
+  <si>
+    <t>Suite 1B, Leeds Innovation Centre 103 Clarendon Road Leeds West Yorkshire LS2 9DF UK</t>
+  </si>
+  <si>
+    <t>LE11 5RG Leicestershire</t>
+  </si>
+  <si>
+    <t>TR18 5HW Cornwall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Innovation Centre Keckwick Lane Daresbury Cheshire WA4 4FS United Kingdom</t>
+  </si>
+  <si>
+    <t>117 Codicote Road Welwyn Hertfordshire AL6 9TY UK</t>
+  </si>
+  <si>
+    <t>181 Harrison Hughes Building School Of Engineering Merseyside L69 3GH UK</t>
+  </si>
+  <si>
+    <t>CV34 5DA Warwickshire</t>
+  </si>
+  <si>
+    <t>CV4 8AF West Midlands</t>
+  </si>
+  <si>
+    <t>CA1 2SQ Cumbria</t>
+  </si>
+  <si>
+    <t>G12 8QQ Glasgow City</t>
+  </si>
+  <si>
+    <t>College Business Park Kearsley Road Ripon North Yorkshire HG4 2RN UK</t>
+  </si>
+  <si>
+    <t>Snaygill Industrial Estate Keighley Road Skipton North Yorkshire BD23 2QR UK</t>
+  </si>
+  <si>
+    <t>AL5 2TL Hertfordshire</t>
+  </si>
+  <si>
+    <t>TF1 7YU Shropshire</t>
+  </si>
+  <si>
+    <t>Unit 10, Charnwood Business Park North Road Loughborough Leicestershire LE11 1QJ UK</t>
+  </si>
+  <si>
+    <t>The Hexagon Theatre Queens Walk Reading RG1 7UA UK</t>
+  </si>
+  <si>
+    <t>BS16 7FR Bristol</t>
+  </si>
+  <si>
+    <t>CV21 1ST Warwickshire</t>
+  </si>
+  <si>
+    <t>CV10 0TU Warwickshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit7 RawdonNetworkCentre MarquisDrive Moira, Leicestershire DE12 6EJ </t>
+  </si>
+  <si>
+    <t>GL6 0JF Gloucestershire</t>
+  </si>
+  <si>
+    <t>S60 5BL South Yorkshire</t>
+  </si>
+  <si>
+    <t>OL10 2TT Greater Manchester</t>
+  </si>
+  <si>
+    <t>SW7 2AZ City of London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polaris House North Star Avenue Swindon Wiltshire SN2 1FL </t>
+  </si>
+  <si>
+    <t>TF7 4NY Shropshire</t>
+  </si>
+  <si>
+    <t>CB24 4UQ Cambridgeshire</t>
+  </si>
+  <si>
+    <t>bb7 4qb Lancashire</t>
+  </si>
+  <si>
+    <t>NG7 7HL Nottinghamshire</t>
+  </si>
+  <si>
+    <t>Coppice Lane Aldridge West Midlands West Midlands WS9 9AA UK</t>
+  </si>
+  <si>
+    <t>Quay Lane Gosport PO12 4LB United Kingdom</t>
+  </si>
+  <si>
+    <t>S80 2PU Nottinghamshire</t>
+  </si>
+  <si>
+    <t>OX28 4FA Oxfordshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 9, The Felbridge Centre East Grinstead West Sussex RH19 1XP </t>
+  </si>
+  <si>
+    <t>51 Clarkegrove Road Shiffield South Yorkshire S10 2NH United Kingdom</t>
+  </si>
+  <si>
+    <t>ST6 6AS Staffordshire</t>
+  </si>
+  <si>
+    <t>AL5 5BZ Hertfordshire</t>
+  </si>
+  <si>
+    <t>1A Bankwood Industrial Estate Bankwood Lane Doncaster DN11 0PS United Kingdom</t>
+  </si>
+  <si>
+    <t>Capital Court, 42 Ffordd William Morgan St. Asaph Business Park St. Asaph Denbighshire LL17 0JG UK</t>
+  </si>
+  <si>
+    <t>DE74 2SA Leicestershire</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>WS10 9LL West Midlands</t>
+  </si>
+  <si>
+    <t>CV21 1PB Warwickshire</t>
+  </si>
+  <si>
+    <t>MK43 0AL Bedfordshire</t>
+  </si>
+  <si>
+    <t>Dennis Road Widnes WA8 0GU United Kingdom</t>
+  </si>
+  <si>
+    <t>ST4 7LQ Staffordshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rutledge House 78 Clarkehouse Road Sheffield S10 2LJ </t>
+  </si>
+  <si>
+    <t>M43 7AJ Greater Manchester</t>
+  </si>
+  <si>
+    <t>WR4 9GN Worcestershire</t>
+  </si>
+  <si>
+    <t>Gee Road Whitwick Business Park Coalville Leicestershire LE67 4NH United Kingdom</t>
+  </si>
+  <si>
+    <t>WR4 9NF Worcestershire</t>
+  </si>
+  <si>
+    <t>CB21 4XN Cambridgeshire</t>
+  </si>
+  <si>
+    <t>Unit 2, Farfield Park, Manvers Way, Wath upon Dearne, Rotherham S63 5DB United Kingdom</t>
+  </si>
+  <si>
+    <t>WR14 1QD Worcestershire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit E18 Langham Park Lows Lane Ilkeston Derbyshire De74RJ </t>
+  </si>
+  <si>
+    <t>SG5 3JH Hertfordshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Archipelago Lyon Way Frimley Surrey GU16 7ER </t>
+  </si>
+  <si>
+    <t>B98 0DG Worcestershire</t>
+  </si>
+  <si>
+    <t>EX31 1GE Devon</t>
+  </si>
+  <si>
+    <t>S9 1XU United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FeynmanWayCentral Bristol&amp;BathSciencePark EmersonsGreen Bristol, BS167FS BS16 7FS </t>
+  </si>
+  <si>
+    <t>424 Argosy Road East Midlands Airport,Castle Donington Derby Derbyshire DE74 2SA UK</t>
+  </si>
+  <si>
+    <t>CA11 9BQ Cumbria</t>
+  </si>
+  <si>
+    <t>HP12 3SY Buckinghamshire</t>
+  </si>
+  <si>
+    <t>BB1 3NY Lancashire</t>
+  </si>
+  <si>
+    <t>SG6 1JA Hertfordshire</t>
+  </si>
+  <si>
+    <t>SS2 5QH Essex</t>
+  </si>
+  <si>
+    <t>Bristol Robotics Laboratory Filton Bristol Avon &amp; Somerset BS16 1QY UK</t>
+  </si>
+  <si>
+    <t>The Yard Old Crown Lane Brentwood Essex CM14 5TA UK</t>
+  </si>
+  <si>
+    <t>SS14 3BY Essex</t>
+  </si>
+  <si>
+    <t>OX5 1PF Oxfordshire</t>
+  </si>
+  <si>
+    <t>OX1 2JD Oxfordshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AviationWay DurhamTeesValleyAirport Darlington CountyDurham DL2 1NA </t>
+  </si>
+  <si>
+    <t>_x005F_x000D_United Kingdom Hertford Unit 2-3 Priory Wharf Priory Street United Kingdom</t>
+  </si>
+  <si>
+    <t>Western Avenue Cardiff CF5 2YB UK</t>
+  </si>
+  <si>
+    <t>14 Kirkpatrick Court Dumfries Scotland DG2 7DG UK</t>
+  </si>
+  <si>
+    <t>BN27 3JU East Sussex</t>
+  </si>
+  <si>
+    <t>Cambridge House Oxney Road Peterborough PE1 5YW UK</t>
+  </si>
+  <si>
+    <t>GL2 2AT Gloucestershire</t>
+  </si>
+  <si>
+    <t>26 Chase Road Park Roya London NW10 6BB UK</t>
+  </si>
+  <si>
+    <t>NN4 7YL Northamptonshire</t>
+  </si>
+  <si>
+    <t>BN1 9PZ East Sussex</t>
+  </si>
+  <si>
+    <t>The Old Fire Station Pandy Park Aberkenfig Brigend CF32 9RE UK</t>
+  </si>
+  <si>
+    <t>CB6 1RA Cambridgeshire</t>
+  </si>
+  <si>
+    <t>28 Britton Street London EC1M 5UE UK</t>
+  </si>
+  <si>
+    <t>64 Thoroughfare Woodbridge Suffolk IP12 1AL UK</t>
+  </si>
+  <si>
+    <t>RG14 5TS Berkshire</t>
+  </si>
+  <si>
+    <t>Maryport Business Centre Main Road Maryport Cumbria CA15 8NG UK</t>
+  </si>
+  <si>
+    <t>130 Wilbury Rd Letchworth Garden City Hertfordshire SG6 4JG United Kingdom</t>
+  </si>
+  <si>
+    <t>Castle Lane Melbourne Derbyshire DE73 8JB UK</t>
+  </si>
+  <si>
+    <t>Bezant House Bradgate Park View Chellaston Derby DE73 5UH United KIngdom</t>
+  </si>
+  <si>
+    <t>Units 19 &amp; 20, Whitworth Road Armstrong Industrial Estate Washington Tyne &amp; Wear NE37 1PR UK</t>
+  </si>
+  <si>
+    <t>BS1 6QA Bristol</t>
+  </si>
+  <si>
+    <t>PE19 6YH Cambridgeshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NewMills Wotton-under-Edge Gloucestershire GL12 8JR </t>
+  </si>
+  <si>
+    <t>S33 6RB Derbyshire</t>
+  </si>
+  <si>
+    <t>Unit 434, Birch Park Thorp Arch Estate Wetherby North Yorkshire LS23 7FG UK</t>
+  </si>
+  <si>
+    <t>M14 7LU Greater Manchester</t>
+  </si>
+  <si>
+    <t>HP22 5BH Buckinghamshire</t>
+  </si>
+  <si>
+    <t>TW13 7EW City of London</t>
+  </si>
+  <si>
+    <t>BS30 8XG Gloucestershire</t>
+  </si>
+  <si>
+    <t>Red Jacket Works Milland Road Neath South Wales SA11 1NJ UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Foundry Place Towcester Northamptonshire NN12 6FP </t>
+  </si>
+  <si>
+    <t>EH54 5DL West Lothian</t>
+  </si>
+  <si>
+    <t>ST12 9HP Staffordshire</t>
+  </si>
+  <si>
+    <t>CH65 3EN Cheshire</t>
+  </si>
+  <si>
+    <t>Baldwin Road Stourport on Severn Worcestershire DY13 9AX UK</t>
+  </si>
+  <si>
+    <t>B29 6EY West Midlands</t>
+  </si>
+  <si>
+    <t>Unit 2, Hatch Industrial Park Greywell Road Mapledurwell Hampshire RG24 7NG UK</t>
+  </si>
+  <si>
+    <t>IG8 9RS City of London</t>
+  </si>
+  <si>
+    <t>CV3 4FG West Midlands</t>
+  </si>
+  <si>
+    <t>LL13 9UZ Wrexham</t>
+  </si>
+  <si>
+    <t>SO17 1BJ Hampshire</t>
+  </si>
+  <si>
+    <t>_x005F_x000D_United Kingdom Scotland The Whisky Bond 2 Dawson Road Glasgow United Kingdom</t>
+  </si>
+  <si>
+    <t>DE56 0RN Derbyshire</t>
+  </si>
+  <si>
+    <t>TR27 6DS Cornwall</t>
+  </si>
+  <si>
+    <t>Faraday House Woodyard Lane Foston Derbyshire DE65 5BU UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit1 14CamphillIndustrialEstate WestByfleet Surrey KT14 6EW </t>
+  </si>
+  <si>
+    <t>NG8 1BB Nottinghamshire</t>
+  </si>
+  <si>
+    <t>River Mill Staveley Mill Yard Staveley Cumbria LA8 9LR UK</t>
+  </si>
+  <si>
+    <t>Pilot Way Ansty Park Coventry CV7 9JU UK</t>
+  </si>
+  <si>
+    <t>130 wilbury road letchworth Herts SG6 4JG UK</t>
+  </si>
+  <si>
+    <t>Malvern Rd Cheltenham  GL50 2NS United Kingdom</t>
+  </si>
+  <si>
+    <t>RH1 5DZ Surrey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-4InnovationWay NorthStaffsBusinessPark StokeonTrent Staffordshire ST6 4BF </t>
+  </si>
+  <si>
+    <t>President Way Luton Bedfordshire LU2 9NL UK</t>
+  </si>
+  <si>
+    <t>CB21 6AL Cambridgeshire</t>
+  </si>
+  <si>
+    <t>GU3 1LR Surrey</t>
+  </si>
+  <si>
+    <t>Bradford BD7 1DP United Kingdom</t>
+  </si>
+  <si>
+    <t>KEDLESTON ROAD DERBY DERBYSHIRE DE22 1GB UNITED KINGDOM</t>
+  </si>
+  <si>
+    <t>Innovation Park Triumph Road Nottingham NG7 2TU UK</t>
+  </si>
+  <si>
+    <t>School Engineering Mi Building, City Campus South Wulfruna Street  Wolverhampton  Wv1 1ly United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Business Park Pavilion Way Loughborough Leicestershire LE11 5GW </t>
+  </si>
+  <si>
+    <t>SL6 1AP Buckinghamshire</t>
+  </si>
+  <si>
+    <t>B63 2RR West Midlands</t>
+  </si>
+  <si>
+    <t>B69 2BN West Midlands</t>
+  </si>
+  <si>
+    <t>MK8 0AB Buckinghamshire</t>
+  </si>
+  <si>
+    <t>Sunderland Software Centre, Tavistock Place Sunderland SR1 1PB Poland</t>
+  </si>
+  <si>
+    <t>B7 4SL West Midlands</t>
+  </si>
+  <si>
+    <t>11 Fenton Way Basildon SS15 6LY United KIngdom</t>
+  </si>
+  <si>
+    <t>TR16 4AX Cornwall</t>
+  </si>
+  <si>
+    <t>OX16 3JU Oxfordshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Meadow Street Sheffield S3 7BL </t>
+  </si>
+  <si>
+    <t>Whitnick Business Park  Coalville   LE67 4JP United Kingdom</t>
+  </si>
+  <si>
+    <t>University of Warwick International Manufacturing Centre Coventry United Kingdom CV4 7AL United Kingdom</t>
+  </si>
+  <si>
+    <t>DE65 5BU Derbyshire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5718,29 +6528,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M277"/>
+  <dimension ref="A1:N277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="28.41796875" customWidth="1"/>
-    <col min="3" max="3" width="24.41796875" customWidth="1"/>
-    <col min="4" max="4" width="20.41796875" customWidth="1"/>
-    <col min="5" max="5" width="74.68359375" customWidth="1"/>
-    <col min="6" max="6" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.578125" customWidth="1"/>
-    <col min="8" max="8" width="25.578125" customWidth="1"/>
-    <col min="9" max="9" width="31.41796875" customWidth="1"/>
-    <col min="10" max="10" width="4.578125" customWidth="1"/>
-    <col min="11" max="12" width="4.83984375" customWidth="1"/>
-    <col min="13" max="13" width="36.68359375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="25.5" customWidth="1"/>
+    <col min="9" max="9" width="31.5" customWidth="1"/>
+    <col min="10" max="10" width="4.5" customWidth="1"/>
+    <col min="11" max="12" width="4.83203125" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="86.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5780,8 +6591,11 @@
       <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5821,8 +6635,11 @@
       <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5862,8 +6679,11 @@
       <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5903,8 +6723,11 @@
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5944,8 +6767,11 @@
       <c r="M5" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5985,8 +6811,11 @@
       <c r="M6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6026,8 +6855,11 @@
       <c r="M7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -6067,8 +6899,11 @@
       <c r="M8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -6108,8 +6943,11 @@
       <c r="M9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -6149,8 +6987,11 @@
       <c r="M10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -6190,8 +7031,11 @@
       <c r="M11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -6231,8 +7075,11 @@
       <c r="M12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -6272,8 +7119,11 @@
       <c r="M13" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -6313,8 +7163,11 @@
       <c r="M14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -6354,8 +7207,11 @@
       <c r="M15" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -6395,8 +7251,11 @@
       <c r="M16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6436,8 +7295,11 @@
       <c r="M17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6477,8 +7339,11 @@
       <c r="M18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6518,8 +7383,11 @@
       <c r="M19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6559,8 +7427,11 @@
       <c r="M20" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -6600,8 +7471,11 @@
       <c r="M21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -6641,8 +7515,11 @@
       <c r="M22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -6682,8 +7559,11 @@
       <c r="M23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6723,8 +7603,11 @@
       <c r="M24" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6764,8 +7647,11 @@
       <c r="M25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6805,8 +7691,11 @@
       <c r="M26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6846,8 +7735,11 @@
       <c r="M27" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6887,8 +7779,11 @@
       <c r="M28" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6928,8 +7823,11 @@
       <c r="M29" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6969,8 +7867,11 @@
       <c r="M30" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7010,8 +7911,11 @@
       <c r="M31" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -7051,8 +7955,11 @@
       <c r="M32" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -7092,8 +7999,11 @@
       <c r="M33" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -7133,8 +8043,11 @@
       <c r="M34" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -7174,8 +8087,11 @@
       <c r="M35" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -7215,8 +8131,11 @@
       <c r="M36" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -7256,8 +8175,11 @@
       <c r="M37" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -7297,8 +8219,11 @@
       <c r="M38" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -7338,8 +8263,11 @@
       <c r="M39" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -7379,8 +8307,11 @@
       <c r="M40" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -7420,8 +8351,11 @@
       <c r="M41" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -7461,8 +8395,11 @@
       <c r="M42" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -7502,8 +8439,11 @@
       <c r="M43" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -7543,8 +8483,11 @@
       <c r="M44" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -7584,8 +8527,11 @@
       <c r="M45" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7625,8 +8571,11 @@
       <c r="M46" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -7666,8 +8615,11 @@
       <c r="M47" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -7707,8 +8659,11 @@
       <c r="M48" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -7748,8 +8703,11 @@
       <c r="M49" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7789,8 +8747,11 @@
       <c r="M50" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="N50" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7830,8 +8791,11 @@
       <c r="M51" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7871,8 +8835,11 @@
       <c r="M52" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -7912,8 +8879,11 @@
       <c r="M53" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -7953,8 +8923,11 @@
       <c r="M54" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -7994,8 +8967,11 @@
       <c r="M55" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -8035,8 +9011,11 @@
       <c r="M56" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -8076,8 +9055,11 @@
       <c r="M57" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -8118,7 +9100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -8158,8 +9140,11 @@
       <c r="M59" s="2" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -8199,8 +9184,11 @@
       <c r="M60" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -8240,8 +9228,11 @@
       <c r="M61" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -8281,8 +9272,11 @@
       <c r="M62" s="2" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -8322,8 +9316,11 @@
       <c r="M63" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -8363,8 +9360,11 @@
       <c r="M64" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -8404,8 +9404,11 @@
       <c r="M65" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -8445,8 +9448,11 @@
       <c r="M66" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -8486,8 +9492,11 @@
       <c r="M67" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -8527,8 +9536,11 @@
       <c r="M68" s="2" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -8568,8 +9580,11 @@
       <c r="M69" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -8609,8 +9624,11 @@
       <c r="M70" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="N70" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -8650,8 +9668,11 @@
       <c r="M71" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N71" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8691,8 +9712,11 @@
       <c r="M72" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="N72" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -8729,8 +9753,11 @@
       <c r="M73" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="N73" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -8770,8 +9797,11 @@
       <c r="M74" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="N74" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8811,8 +9841,11 @@
       <c r="M75" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8852,8 +9885,11 @@
       <c r="M76" s="2" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8893,8 +9929,11 @@
       <c r="M77" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="N77" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8931,8 +9970,11 @@
       <c r="M78" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="N78" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8972,8 +10014,11 @@
       <c r="M79" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -9013,8 +10058,11 @@
       <c r="M80" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -9054,8 +10102,11 @@
       <c r="M81" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -9095,8 +10146,11 @@
       <c r="M82" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -9136,8 +10190,11 @@
       <c r="M83" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -9177,8 +10234,11 @@
       <c r="M84" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="N84" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -9218,8 +10278,11 @@
       <c r="M85" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="N85" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -9259,8 +10322,11 @@
       <c r="M86" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="N86" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -9300,8 +10366,11 @@
       <c r="M87" s="2" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="N87" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -9341,8 +10410,11 @@
       <c r="M88" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="N88" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -9379,8 +10451,11 @@
       <c r="M89" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="N89" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -9420,8 +10495,11 @@
       <c r="M90" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" ht="57.6">
+      <c r="N90" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -9461,8 +10539,11 @@
       <c r="M91" s="2" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="N91" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -9502,8 +10583,11 @@
       <c r="M92" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="N92" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -9543,8 +10627,11 @@
       <c r="M93" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="N93" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -9584,8 +10671,11 @@
       <c r="M94" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="N94" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -9625,8 +10715,11 @@
       <c r="M95" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="N95" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -9666,8 +10759,11 @@
       <c r="M96" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="N96" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -9707,8 +10803,11 @@
       <c r="M97" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="N97" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -9748,8 +10847,11 @@
       <c r="M98" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="N98" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -9789,8 +10891,11 @@
       <c r="M99" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="N99" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9830,8 +10935,11 @@
       <c r="M100" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="N100" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9871,8 +10979,11 @@
       <c r="M101" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="N101" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9912,8 +11023,11 @@
       <c r="M102" s="2" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="N102" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9953,8 +11067,11 @@
       <c r="M103" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="N103" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9994,8 +11111,11 @@
       <c r="M104" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="N104" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -10035,8 +11155,11 @@
       <c r="M105" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="N105" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -10076,8 +11199,11 @@
       <c r="M106" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="N106" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -10117,8 +11243,11 @@
       <c r="M107" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" ht="28.8">
+      <c r="N107" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -10158,8 +11287,11 @@
       <c r="M108" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="N108" t="s">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -10199,8 +11331,11 @@
       <c r="M109" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="N109" t="s">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -10240,8 +11375,11 @@
       <c r="M110" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="N110" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -10281,8 +11419,11 @@
       <c r="M111" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="N111" t="s">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -10322,8 +11463,11 @@
       <c r="M112" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="N112" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -10363,8 +11507,11 @@
       <c r="M113" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="114" spans="1:13">
+      <c r="N113" t="s">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -10404,8 +11551,11 @@
       <c r="M114" s="2" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="N114" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -10445,8 +11595,11 @@
       <c r="M115" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="N115" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -10486,8 +11639,11 @@
       <c r="M116" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="N116" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -10527,8 +11683,11 @@
       <c r="M117" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="N117" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -10568,8 +11727,11 @@
       <c r="M118" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="119" spans="1:13">
+      <c r="N118" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -10609,8 +11771,11 @@
       <c r="M119" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="120" spans="1:13">
+      <c r="N119" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -10650,8 +11815,11 @@
       <c r="M120" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="121" spans="1:13">
+      <c r="N120" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -10691,8 +11859,11 @@
       <c r="M121" s="2" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="122" spans="1:13">
+      <c r="N121" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -10732,8 +11903,11 @@
       <c r="M122" s="2" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="123" spans="1:13">
+      <c r="N122" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -10773,8 +11947,11 @@
       <c r="M123" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="124" spans="1:13">
+      <c r="N123" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -10814,8 +11991,11 @@
       <c r="M124" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="125" spans="1:13">
+      <c r="N124" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -10855,8 +12035,11 @@
       <c r="M125" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="126" spans="1:13">
+      <c r="N125" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -10896,8 +12079,11 @@
       <c r="M126" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="127" spans="1:13">
+      <c r="N126" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -10937,8 +12123,11 @@
       <c r="M127" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="128" spans="1:13">
+      <c r="N127" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -10978,8 +12167,11 @@
       <c r="M128" s="2" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="129" spans="1:13">
+      <c r="N128" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -11019,8 +12211,11 @@
       <c r="M129" s="2" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="130" spans="1:13">
+      <c r="N129" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -11060,8 +12255,11 @@
       <c r="M130" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="131" spans="1:13">
+      <c r="N130" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -11101,8 +12299,11 @@
       <c r="M131" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="132" spans="1:13">
+      <c r="N131" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -11142,8 +12343,11 @@
       <c r="M132" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="133" spans="1:13">
+      <c r="N132" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -11183,8 +12387,11 @@
       <c r="M133" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="134" spans="1:13">
+      <c r="N133" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -11224,8 +12431,11 @@
       <c r="M134" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="135" spans="1:13">
+      <c r="N134" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -11265,8 +12475,11 @@
       <c r="M135" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="136" spans="1:13">
+      <c r="N135" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -11306,8 +12519,11 @@
       <c r="M136" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="137" spans="1:13">
+      <c r="N136" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -11347,8 +12563,11 @@
       <c r="M137" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="138" spans="1:13">
+      <c r="N137" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -11388,8 +12607,11 @@
       <c r="M138" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="139" spans="1:13">
+      <c r="N138" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -11429,8 +12651,11 @@
       <c r="M139" s="2" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="140" spans="1:13">
+      <c r="N139" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -11470,8 +12695,11 @@
       <c r="M140" s="2" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="141" spans="1:13">
+      <c r="N140" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -11512,7 +12740,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -11549,8 +12777,11 @@
       <c r="M142" s="2" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="143" spans="1:13">
+      <c r="N142" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -11590,8 +12821,11 @@
       <c r="M143" s="2" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="144" spans="1:13">
+      <c r="N143" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -11631,8 +12865,11 @@
       <c r="M144" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="145" spans="1:13">
+      <c r="N144" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -11672,8 +12909,11 @@
       <c r="M145" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="146" spans="1:13">
+      <c r="N145" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -11713,8 +12953,11 @@
       <c r="M146" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" ht="28.8">
+      <c r="N146" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -11754,8 +12997,11 @@
       <c r="M147" s="2" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="148" spans="1:13">
+      <c r="N147" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -11795,8 +13041,11 @@
       <c r="M148" s="2" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="149" spans="1:13">
+      <c r="N148" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -11836,8 +13085,11 @@
       <c r="M149" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="150" spans="1:13">
+      <c r="N149" t="s">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -11877,8 +13129,11 @@
       <c r="M150" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="151" spans="1:13">
+      <c r="N150" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -11918,8 +13173,11 @@
       <c r="M151" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="152" spans="1:13">
+      <c r="N151" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -11959,8 +13217,11 @@
       <c r="M152" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="153" spans="1:13">
+      <c r="N152" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -12000,8 +13261,11 @@
       <c r="M153" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="154" spans="1:13">
+      <c r="N153" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -12041,8 +13305,11 @@
       <c r="M154" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="155" spans="1:13">
+      <c r="N154" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -12082,8 +13349,11 @@
       <c r="M155" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="156" spans="1:13">
+      <c r="N155" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -12123,8 +13393,11 @@
       <c r="M156" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="157" spans="1:13">
+      <c r="N156" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -12164,8 +13437,11 @@
       <c r="M157" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="158" spans="1:13">
+      <c r="N157" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -12205,8 +13481,11 @@
       <c r="M158" s="2" t="s">
         <v>1042</v>
       </c>
-    </row>
-    <row r="159" spans="1:13">
+      <c r="N158" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -12246,8 +13525,11 @@
       <c r="M159" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="160" spans="1:13">
+      <c r="N159" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -12287,8 +13569,11 @@
       <c r="M160" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="161" spans="1:13">
+      <c r="N160" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -12328,8 +13613,11 @@
       <c r="M161" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="162" spans="1:13">
+      <c r="N161" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -12369,8 +13657,11 @@
       <c r="M162" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="163" spans="1:13">
+      <c r="N162" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -12410,8 +13701,11 @@
       <c r="M163" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="164" spans="1:13">
+      <c r="N163" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -12451,8 +13745,11 @@
       <c r="M164" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="165" spans="1:13">
+      <c r="N164" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -12492,8 +13789,11 @@
       <c r="M165" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="166" spans="1:13">
+      <c r="N165" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -12533,8 +13833,11 @@
       <c r="M166" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="167" spans="1:13">
+      <c r="N166" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -12574,8 +13877,11 @@
       <c r="M167" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="168" spans="1:13">
+      <c r="N167" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -12615,8 +13921,11 @@
       <c r="M168" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="169" spans="1:13">
+      <c r="N168" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -12656,8 +13965,11 @@
       <c r="M169" s="2" t="s">
         <v>1110</v>
       </c>
-    </row>
-    <row r="170" spans="1:13">
+      <c r="N169" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -12697,8 +14009,11 @@
       <c r="M170" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="171" spans="1:13">
+      <c r="N170" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -12738,8 +14053,11 @@
       <c r="M171" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="172" spans="1:13">
+      <c r="N171" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -12779,8 +14097,11 @@
       <c r="M172" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="173" spans="1:13">
+      <c r="N172" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -12820,8 +14141,11 @@
       <c r="M173" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="174" spans="1:13" ht="28.8">
+      <c r="N173" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -12861,8 +14185,11 @@
       <c r="M174" s="2" t="s">
         <v>1145</v>
       </c>
-    </row>
-    <row r="175" spans="1:13">
+      <c r="N174" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -12902,8 +14229,11 @@
       <c r="M175" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="176" spans="1:13">
+      <c r="N175" t="s">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -12943,8 +14273,11 @@
       <c r="M176" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="177" spans="1:13">
+      <c r="N176" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -12984,8 +14317,11 @@
       <c r="M177" s="2" t="s">
         <v>1165</v>
       </c>
-    </row>
-    <row r="178" spans="1:13">
+      <c r="N177" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -13025,8 +14361,11 @@
       <c r="M178" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="179" spans="1:13">
+      <c r="N178" t="s">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -13066,8 +14405,11 @@
       <c r="M179" s="2" t="s">
         <v>1179</v>
       </c>
-    </row>
-    <row r="180" spans="1:13">
+      <c r="N179" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -13107,8 +14449,11 @@
       <c r="M180" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="181" spans="1:13">
+      <c r="N180" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -13148,8 +14493,11 @@
       <c r="M181" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="182" spans="1:13">
+      <c r="N181" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -13189,8 +14537,11 @@
       <c r="M182" s="2" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="183" spans="1:13">
+      <c r="N182" t="s">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="183" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -13230,8 +14581,11 @@
       <c r="M183" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="184" spans="1:13">
+      <c r="N183" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="184" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -13271,8 +14625,11 @@
       <c r="M184" s="2" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="185" spans="1:13">
+      <c r="N184" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -13312,8 +14669,11 @@
       <c r="M185" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="186" spans="1:13">
+      <c r="N185" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="186" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -13353,8 +14713,11 @@
       <c r="M186" s="2" t="s">
         <v>1226</v>
       </c>
-    </row>
-    <row r="187" spans="1:13">
+      <c r="N186" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="187" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -13394,8 +14757,11 @@
       <c r="M187" s="2" t="s">
         <v>1233</v>
       </c>
-    </row>
-    <row r="188" spans="1:13">
+      <c r="N187" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -13435,8 +14801,11 @@
       <c r="M188" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="189" spans="1:13">
+      <c r="N188" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -13476,8 +14845,11 @@
       <c r="M189" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="190" spans="1:13">
+      <c r="N189" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -13517,8 +14889,11 @@
       <c r="M190" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="191" spans="1:13">
+      <c r="N190" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -13558,8 +14933,11 @@
       <c r="M191" s="2" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="192" spans="1:13">
+      <c r="N191" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -13599,8 +14977,11 @@
       <c r="M192" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="193" spans="1:13">
+      <c r="N192" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -13640,8 +15021,11 @@
       <c r="M193" s="2" t="s">
         <v>845</v>
       </c>
-    </row>
-    <row r="194" spans="1:13">
+      <c r="N193" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -13681,8 +15065,11 @@
       <c r="M194" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="195" spans="1:13">
+      <c r="N194" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -13722,8 +15109,11 @@
       <c r="M195" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="196" spans="1:13">
+      <c r="N195" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -13763,8 +15153,11 @@
       <c r="M196" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="197" spans="1:13">
+      <c r="N196" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -13804,8 +15197,11 @@
       <c r="M197" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="198" spans="1:13">
+      <c r="N197" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -13845,8 +15241,11 @@
       <c r="M198" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="199" spans="1:13">
+      <c r="N198" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="199" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -13886,8 +15285,11 @@
       <c r="M199" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="200" spans="1:13" ht="28.8">
+      <c r="N199" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -13927,8 +15329,11 @@
       <c r="M200" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="201" spans="1:13">
+      <c r="N200" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="201" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -13968,8 +15373,11 @@
       <c r="M201" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="202" spans="1:13">
+      <c r="N201" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="202" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -14009,8 +15417,11 @@
       <c r="M202" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="203" spans="1:13">
+      <c r="N202" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -14050,8 +15461,11 @@
       <c r="M203" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="204" spans="1:13">
+      <c r="N203" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -14091,8 +15505,11 @@
       <c r="M204" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="205" spans="1:13">
+      <c r="N204" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -14132,8 +15549,11 @@
       <c r="M205" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="206" spans="1:13">
+      <c r="N205" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -14173,8 +15593,11 @@
       <c r="M206" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="207" spans="1:13">
+      <c r="N206" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -14214,8 +15637,11 @@
       <c r="M207" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="208" spans="1:13" ht="28.8">
+      <c r="N207" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -14255,8 +15681,11 @@
       <c r="M208" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="209" spans="1:13">
+      <c r="N208" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
@@ -14296,8 +15725,11 @@
       <c r="M209" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="210" spans="1:13">
+      <c r="N209" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
@@ -14334,8 +15766,11 @@
       <c r="M210" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="211" spans="1:13">
+      <c r="N210" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
@@ -14372,8 +15807,11 @@
       <c r="M211" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="212" spans="1:13">
+      <c r="N211" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>211</v>
       </c>
@@ -14413,8 +15851,11 @@
       <c r="M212" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="213" spans="1:13">
+      <c r="N212" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
@@ -14454,8 +15895,11 @@
       <c r="M213" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="214" spans="1:13">
+      <c r="N213" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
@@ -14495,8 +15939,11 @@
       <c r="M214" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="215" spans="1:13">
+      <c r="N214" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
@@ -14536,8 +15983,11 @@
       <c r="M215" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="216" spans="1:13">
+      <c r="N215" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>215</v>
       </c>
@@ -14577,8 +16027,11 @@
       <c r="M216" s="2" t="s">
         <v>1401</v>
       </c>
-    </row>
-    <row r="217" spans="1:13">
+      <c r="N216" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>216</v>
       </c>
@@ -14618,8 +16071,11 @@
       <c r="M217" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="218" spans="1:13">
+      <c r="N217" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="218" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>217</v>
       </c>
@@ -14659,8 +16115,11 @@
       <c r="M218" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="219" spans="1:13">
+      <c r="N218" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>218</v>
       </c>
@@ -14700,8 +16159,11 @@
       <c r="M219" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="220" spans="1:13">
+      <c r="N219" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>219</v>
       </c>
@@ -14738,8 +16200,11 @@
       <c r="M220" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="221" spans="1:13">
+      <c r="N220" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>220</v>
       </c>
@@ -14779,8 +16244,11 @@
       <c r="M221" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="222" spans="1:13">
+      <c r="N221" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>221</v>
       </c>
@@ -14820,8 +16288,11 @@
       <c r="M222" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="223" spans="1:13">
+      <c r="N222" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>222</v>
       </c>
@@ -14861,8 +16332,11 @@
       <c r="M223" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="224" spans="1:13">
+      <c r="N223" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>223</v>
       </c>
@@ -14902,8 +16376,11 @@
       <c r="M224" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="225" spans="1:13">
+      <c r="N224" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>224</v>
       </c>
@@ -14943,8 +16420,11 @@
       <c r="M225" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="226" spans="1:13">
+      <c r="N225" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>225</v>
       </c>
@@ -14984,8 +16464,11 @@
       <c r="M226" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="227" spans="1:13">
+      <c r="N226" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>226</v>
       </c>
@@ -15025,8 +16508,11 @@
       <c r="M227" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="228" spans="1:13">
+      <c r="N227" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>227</v>
       </c>
@@ -15066,8 +16552,11 @@
       <c r="M228" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="229" spans="1:13">
+      <c r="N228" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>228</v>
       </c>
@@ -15107,8 +16596,11 @@
       <c r="M229" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="230" spans="1:13" ht="28.8">
+      <c r="N229" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>229</v>
       </c>
@@ -15148,8 +16640,11 @@
       <c r="M230" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="231" spans="1:13">
+      <c r="N230" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>230</v>
       </c>
@@ -15189,8 +16684,11 @@
       <c r="M231" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="232" spans="1:13">
+      <c r="N231" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>231</v>
       </c>
@@ -15230,8 +16728,11 @@
       <c r="M232" s="2" t="s">
         <v>1496</v>
       </c>
-    </row>
-    <row r="233" spans="1:13" ht="28.8">
+      <c r="N232" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>232</v>
       </c>
@@ -15271,8 +16772,11 @@
       <c r="M233" s="2" t="s">
         <v>1503</v>
       </c>
-    </row>
-    <row r="234" spans="1:13">
+      <c r="N233" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>233</v>
       </c>
@@ -15312,8 +16816,11 @@
       <c r="M234" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="235" spans="1:13" ht="28.8">
+      <c r="N234" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>234</v>
       </c>
@@ -15353,8 +16860,11 @@
       <c r="M235" s="2" t="s">
         <v>1515</v>
       </c>
-    </row>
-    <row r="236" spans="1:13">
+      <c r="N235" t="s">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>235</v>
       </c>
@@ -15394,8 +16904,11 @@
       <c r="M236" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="237" spans="1:13">
+      <c r="N236" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>236</v>
       </c>
@@ -15435,8 +16948,11 @@
       <c r="M237" s="2" t="s">
         <v>1528</v>
       </c>
-    </row>
-    <row r="238" spans="1:13">
+      <c r="N237" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>237</v>
       </c>
@@ -15476,8 +16992,11 @@
       <c r="M238" s="2" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="239" spans="1:13">
+      <c r="N238" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>238</v>
       </c>
@@ -15517,8 +17036,11 @@
       <c r="M239" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="240" spans="1:13">
+      <c r="N239" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>239</v>
       </c>
@@ -15558,8 +17080,11 @@
       <c r="M240" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="241" spans="1:13">
+      <c r="N240" t="s">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="241" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>240</v>
       </c>
@@ -15599,8 +17124,11 @@
       <c r="M241" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="242" spans="1:13">
+      <c r="N241" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="242" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>241</v>
       </c>
@@ -15640,8 +17168,11 @@
       <c r="M242" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="243" spans="1:13">
+      <c r="N242" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>242</v>
       </c>
@@ -15681,8 +17212,11 @@
       <c r="M243" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="244" spans="1:13">
+      <c r="N243" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>243</v>
       </c>
@@ -15722,8 +17256,11 @@
       <c r="M244" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="245" spans="1:13">
+      <c r="N244" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="245" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>244</v>
       </c>
@@ -15763,8 +17300,11 @@
       <c r="M245" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="246" spans="1:13" ht="28.8">
+      <c r="N245" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>245</v>
       </c>
@@ -15804,8 +17344,11 @@
       <c r="M246" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="247" spans="1:13" ht="28.8">
+      <c r="N246" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>246</v>
       </c>
@@ -15845,8 +17388,11 @@
       <c r="M247" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="248" spans="1:13">
+      <c r="N247" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>247</v>
       </c>
@@ -15886,8 +17432,11 @@
       <c r="M248" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="249" spans="1:13">
+      <c r="N248" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="249" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>248</v>
       </c>
@@ -15927,8 +17476,11 @@
       <c r="M249" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="250" spans="1:13" ht="28.8">
+      <c r="N249" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="250" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>249</v>
       </c>
@@ -15968,8 +17520,11 @@
       <c r="M250" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="251" spans="1:13">
+      <c r="N250" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>250</v>
       </c>
@@ -16009,8 +17564,11 @@
       <c r="M251" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="252" spans="1:13">
+      <c r="N251" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="252" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>251</v>
       </c>
@@ -16047,8 +17605,11 @@
       <c r="M252" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="253" spans="1:13">
+      <c r="N252" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>252</v>
       </c>
@@ -16088,8 +17649,11 @@
       <c r="M253" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="254" spans="1:13">
+      <c r="N253" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>253</v>
       </c>
@@ -16129,8 +17693,11 @@
       <c r="M254" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="255" spans="1:13">
+      <c r="N254" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="255" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>254</v>
       </c>
@@ -16170,8 +17737,11 @@
       <c r="M255" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="256" spans="1:13">
+      <c r="N255" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>255</v>
       </c>
@@ -16211,8 +17781,11 @@
       <c r="M256" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="257" spans="1:13" ht="28.8">
+      <c r="N256" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="257" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>256</v>
       </c>
@@ -16252,8 +17825,11 @@
       <c r="M257" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="258" spans="1:13">
+      <c r="N257" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>257</v>
       </c>
@@ -16293,8 +17869,11 @@
       <c r="M258" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="259" spans="1:13">
+      <c r="N258" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>258</v>
       </c>
@@ -16334,8 +17913,11 @@
       <c r="M259" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="260" spans="1:13">
+      <c r="N259" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>259</v>
       </c>
@@ -16375,8 +17957,11 @@
       <c r="M260" s="2" t="s">
         <v>1661</v>
       </c>
-    </row>
-    <row r="261" spans="1:13">
+      <c r="N260" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>260</v>
       </c>
@@ -16416,8 +18001,11 @@
       <c r="M261" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="262" spans="1:13">
+      <c r="N261" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>261</v>
       </c>
@@ -16457,8 +18045,11 @@
       <c r="M262" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="263" spans="1:13">
+      <c r="N262" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>262</v>
       </c>
@@ -16498,8 +18089,11 @@
       <c r="M263" s="2" t="s">
         <v>1679</v>
       </c>
-    </row>
-    <row r="264" spans="1:13">
+      <c r="N263" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>263</v>
       </c>
@@ -16539,8 +18133,11 @@
       <c r="M264" s="2" t="s">
         <v>1503</v>
       </c>
-    </row>
-    <row r="265" spans="1:13">
+      <c r="N264" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>264</v>
       </c>
@@ -16580,8 +18177,11 @@
       <c r="M265" s="2" t="s">
         <v>1691</v>
       </c>
-    </row>
-    <row r="266" spans="1:13">
+      <c r="N265" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>265</v>
       </c>
@@ -16621,8 +18221,11 @@
       <c r="M266" s="2" t="s">
         <v>1698</v>
       </c>
-    </row>
-    <row r="267" spans="1:13">
+      <c r="N266" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="267" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>266</v>
       </c>
@@ -16662,8 +18265,11 @@
       <c r="M267" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="268" spans="1:13">
+      <c r="N267" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="268" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>267</v>
       </c>
@@ -16703,8 +18309,11 @@
       <c r="M268" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="269" spans="1:13" ht="28.8">
+      <c r="N268" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="269" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>268</v>
       </c>
@@ -16744,8 +18353,11 @@
       <c r="M269" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="270" spans="1:13">
+      <c r="N269" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="270" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>269</v>
       </c>
@@ -16785,8 +18397,11 @@
       <c r="M270" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="271" spans="1:13" ht="28.8">
+      <c r="N270" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="271" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>270</v>
       </c>
@@ -16826,8 +18441,11 @@
       <c r="M271" s="2" t="s">
         <v>1729</v>
       </c>
-    </row>
-    <row r="272" spans="1:13">
+      <c r="N271" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>271</v>
       </c>
@@ -16867,8 +18485,11 @@
       <c r="M272" s="2" t="s">
         <v>1736</v>
       </c>
-    </row>
-    <row r="273" spans="1:13">
+      <c r="N272" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="273" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>272</v>
       </c>
@@ -16908,8 +18529,11 @@
       <c r="M273" s="2" t="s">
         <v>1742</v>
       </c>
-    </row>
-    <row r="274" spans="1:13">
+      <c r="N273" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="274" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>273</v>
       </c>
@@ -16949,8 +18573,11 @@
       <c r="M274" s="2" t="s">
         <v>1749</v>
       </c>
-    </row>
-    <row r="275" spans="1:13">
+      <c r="N274" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="275" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>274</v>
       </c>
@@ -16990,8 +18617,11 @@
       <c r="M275" s="2" t="s">
         <v>1755</v>
       </c>
-    </row>
-    <row r="276" spans="1:13">
+      <c r="N275" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>275</v>
       </c>
@@ -17031,8 +18661,11 @@
       <c r="M276" s="2" t="s">
         <v>1762</v>
       </c>
-    </row>
-    <row r="277" spans="1:13">
+      <c r="N276" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>276</v>
       </c>
@@ -17071,6 +18704,9 @@
       </c>
       <c r="M277" s="2" t="s">
         <v>200</v>
+      </c>
+      <c r="N277" t="s">
+        <v>2042</v>
       </c>
     </row>
   </sheetData>
@@ -17340,6 +18976,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F21D206E6291634392DF1EE4DEC4486C" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="07cf05e8307afe6a990ed986d433b3b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e5a1dba9-b322-4fe2-a2ac-96a80fc5cb1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f8039b1bbebd6ee1b898fd144949a3bc" ns2:_="">
     <xsd:import namespace="e5a1dba9-b322-4fe2-a2ac-96a80fc5cb1e"/>
@@ -17503,12 +19145,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17519,6 +19155,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A057F9CB-57E5-4529-857B-17E05E15F615}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D937380-67B5-4B64-A0DF-AAB1C6A1371E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17536,15 +19181,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A057F9CB-57E5-4529-857B-17E05E15F615}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F11EC71-C561-409B-A302-C24D3869C13F}">
   <ds:schemaRefs>

</xml_diff>